<commit_message>
LTHDT-LT-Tuan04. Hoan thanh file testcase (2/2).
</commit_message>
<xml_diff>
--- a/LTHDT_LT_Tuan04_PhamThanhTung/demo/LopHP_LT_Tuan04_testcase.xlsx
+++ b/LTHDT_LT_Tuan04_PhamThanhTung/demo/LopHP_LT_Tuan04_testcase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\workspaces\uni_c2023_2024_s1_java_oop_exercises\LTHDT_LT_Tuan04_PhamThanhTung\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3C15E4-9563-49CE-B89A-D952642C7A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7146FE66-B1EA-4C37-B82F-F95516AF900F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="29010" windowHeight="31785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="113">
   <si>
     <t>Passed</t>
   </si>
@@ -394,22 +394,76 @@
     <t>Test cho trường hợp mảng chứa danh sách tài khoản đã đầy</t>
   </si>
   <si>
-    <t>addNew(1001-5555-2050,Cassandra Sirius,7000)</t>
-  </si>
-  <si>
     <t>java.lang.IllegalArgumentException: Bank is full</t>
   </si>
   <si>
     <t>java.lang.IllegalArgumentException: Account number already exists</t>
   </si>
   <si>
-    <t>addNew(1001-5555-2010,Cassandra Sirius,7000)</t>
-  </si>
-  <si>
     <t>Test cho trường hợp mảng chứa danh sách tài khoản chưa đầy và số tài khoản muốn thêm đã tồn tại trong mảng</t>
   </si>
   <si>
     <t>Không có ngoại lệ nào được ném ra</t>
+  </si>
+  <si>
+    <t>addNew(1001-5555-2050,"Cassandra Sirius",7000)</t>
+  </si>
+  <si>
+    <t>addNew(1001-5555-2010,"Cassandra Sirius",7000)</t>
+  </si>
+  <si>
+    <t>Test cho trường hợp tìm được đối tượng thuộc lớp BankAccount</t>
+  </si>
+  <si>
+    <t>Test cho trường hợp không tìm được đối tượng thuộc lớp BankAccount</t>
+  </si>
+  <si>
+    <t>find(1001-5555-2020)</t>
+  </si>
+  <si>
+    <t>find(1001-5555-2021)</t>
+  </si>
+  <si>
+    <t>ownerName="James Edward"</t>
+  </si>
+  <si>
+    <t>ownerName="null"</t>
+  </si>
+  <si>
+    <t>Truy vấn tổng số tiền trong tất cả các tài khoản ngân hàng</t>
+  </si>
+  <si>
+    <t>Truy vấn tên của ngân hàng</t>
+  </si>
+  <si>
+    <t>Hallow Bank</t>
+  </si>
+  <si>
+    <t>Truy vấn danh sách các tài khoản có trong ngân hàng</t>
+  </si>
+  <si>
+    <t>{BankAccount("1001-5555-2010", "Peter Walker", 10000.0), BankAccount("1001-5555-2020","James Edward", 5000.0), BankAccount("1001-5555-2030", "John Smith",8000)}</t>
+  </si>
+  <si>
+    <t>Truy vấn số tài khoản có trong ngân hàng</t>
+  </si>
+  <si>
+    <t>Test cho trường hợp name không rỗng</t>
+  </si>
+  <si>
+    <t>Test cho trường hợp name rỗng</t>
+  </si>
+  <si>
+    <t>name=""</t>
+  </si>
+  <si>
+    <t>name="PI Bank"</t>
+  </si>
+  <si>
+    <t>PI Bank</t>
+  </si>
+  <si>
+    <t>The bank name must not be null</t>
   </si>
 </sst>
 </file>
@@ -577,41 +631,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -626,6 +647,24 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -635,23 +674,38 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -970,47 +1024,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="C31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="92.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="85.08984375" style="1" customWidth="1"/>
     <col min="4" max="4" width="26" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="37.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="40.36328125" style="1" customWidth="1"/>
     <col min="7" max="7" width="34" style="1" customWidth="1"/>
-    <col min="8" max="8" width="34.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="34.54296875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.26953125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" ht="27.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+    </row>
+    <row r="2" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
       <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1019,16 +1073,16 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
       <c r="H3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1037,16 +1091,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
       <c r="H4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1055,7 +1109,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -1084,17 +1138,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
+    <row r="6" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
         <v>1</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="26" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -1113,13 +1167,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
+    <row r="7" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
         <v>2</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="13"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="5" t="s">
         <v>21</v>
       </c>
@@ -1136,13 +1190,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
+    <row r="8" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
         <v>3</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="14"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="28"/>
       <c r="E8" s="5" t="s">
         <v>22</v>
       </c>
@@ -1152,22 +1206,22 @@
       <c r="G8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="8" t="s">
         <v>24</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
         <v>4</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="21"/>
+      <c r="C9" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="26" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -1186,13 +1240,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
+    <row r="10" spans="1:9" ht="39" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
         <v>5</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="13"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="5" t="s">
         <v>21</v>
       </c>
@@ -1209,13 +1263,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+    <row r="11" spans="1:9" ht="39" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
         <v>6</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="13"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="5" t="s">
         <v>22</v>
       </c>
@@ -1232,13 +1286,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22">
+    <row r="12" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
         <v>7</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="14"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="5" t="s">
         <v>33</v>
       </c>
@@ -1255,15 +1309,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="22">
+    <row r="13" spans="1:9" ht="39" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
         <v>8</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="21"/>
+      <c r="C13" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="31" t="s">
         <v>36</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -1275,525 +1329,581 @@
       <c r="G13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="8" t="s">
         <v>41</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="22">
+    <row r="14" spans="1:9" ht="39" x14ac:dyDescent="0.3">
+      <c r="A14" s="11">
         <v>9</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="16"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="31"/>
       <c r="E14" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="24" t="s">
+      <c r="G14" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="H14" s="13" t="s">
         <v>32</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
+    <row r="15" spans="1:9" ht="39" x14ac:dyDescent="0.3">
+      <c r="A15" s="11">
         <v>10</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="16"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="31"/>
       <c r="E15" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="13" t="s">
         <v>32</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22">
+    <row r="16" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11">
         <v>11</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="16"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="31"/>
       <c r="E16" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="24" t="s">
+      <c r="G16" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="13" t="s">
         <v>32</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="39" x14ac:dyDescent="0.25">
-      <c r="A17" s="22">
+    <row r="17" spans="1:9" ht="39" x14ac:dyDescent="0.3">
+      <c r="A17" s="11">
         <v>12</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="28" t="s">
+      <c r="B17" s="21"/>
+      <c r="C17" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="23" t="s">
+      <c r="E17" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="23"/>
-      <c r="G17" s="24">
+      <c r="F17" s="12"/>
+      <c r="G17" s="13">
         <v>10000</v>
       </c>
-      <c r="H17" s="24">
+      <c r="H17" s="13">
         <v>10000</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="39" x14ac:dyDescent="0.25">
-      <c r="A18" s="22">
+    <row r="18" spans="1:9" ht="39" x14ac:dyDescent="0.3">
+      <c r="A18" s="11">
         <v>13</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="28" t="s">
+      <c r="B18" s="21"/>
+      <c r="C18" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23" t="s">
+      <c r="F18" s="12"/>
+      <c r="G18" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="23" t="s">
+      <c r="H18" s="12" t="s">
         <v>53</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="22">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="11">
         <v>14</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="31" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="32" t="s">
+      <c r="D19" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F19" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="24" t="s">
+      <c r="G19" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="13" t="s">
         <v>62</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22">
+    <row r="20" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11">
         <v>15</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="24" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="G20" s="24" t="s">
+      <c r="G20" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H20" s="24" t="s">
+      <c r="H20" s="13" t="s">
         <v>63</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="39" x14ac:dyDescent="0.25">
-      <c r="A21" s="22">
+    <row r="21" spans="1:9" ht="39" x14ac:dyDescent="0.3">
+      <c r="A21" s="11">
         <v>16</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="28" t="s">
+      <c r="B21" s="21"/>
+      <c r="C21" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="23" t="s">
+      <c r="E21" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="23"/>
-      <c r="G21" s="24" t="s">
+      <c r="F21" s="12"/>
+      <c r="G21" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H21" s="24" t="s">
+      <c r="H21" s="13" t="s">
         <v>55</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="22">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="11">
         <v>17</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="31" t="s">
+      <c r="B22" s="21"/>
+      <c r="C22" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="32" t="s">
+      <c r="D22" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="F22" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="G22" s="24" t="s">
+      <c r="G22" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="H22" s="24" t="s">
+      <c r="H22" s="13" t="s">
         <v>59</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22">
+    <row r="23" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11">
         <v>18</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="24" t="s">
+      <c r="B23" s="21"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G23" s="24" t="s">
+      <c r="G23" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H23" s="24" t="s">
+      <c r="H23" s="13" t="s">
         <v>60</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="22">
+    <row r="24" spans="1:9" ht="70" x14ac:dyDescent="0.3">
+      <c r="A24" s="11">
         <v>19</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="20" t="s">
+      <c r="B24" s="22"/>
+      <c r="C24" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="24" t="s">
+      <c r="E24" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="24" t="s">
+      <c r="F24" s="12"/>
+      <c r="G24" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="H24" s="24" t="s">
+      <c r="H24" s="13" t="s">
         <v>70</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="22">
+    <row r="25" spans="1:9" ht="26" x14ac:dyDescent="0.3">
+      <c r="A25" s="11">
         <v>20</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="E25" s="28" t="s">
+      <c r="E25" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F25" s="24" t="s">
+      <c r="F25" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="26" x14ac:dyDescent="0.3">
+      <c r="A26" s="11">
+        <v>21</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G26" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="G25" s="23" t="s">
+      <c r="H26" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="164" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11">
+        <v>22</v>
+      </c>
+      <c r="B27" s="21"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H25" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="22">
-        <v>21</v>
-      </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="F26" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="G26" s="24" t="s">
+      <c r="G27" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="H26" s="24" t="s">
+      <c r="H27" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="I26" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="179.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22">
-        <v>22</v>
-      </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="F27" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="G27" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="H27" s="24" t="s">
-        <v>91</v>
-      </c>
       <c r="I27" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="22">
+    <row r="28" spans="1:9" ht="26" x14ac:dyDescent="0.3">
+      <c r="A28" s="11">
         <v>23</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="31" t="s">
+      <c r="B28" s="21"/>
+      <c r="C28" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="25" t="s">
+      <c r="D28" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="E28" s="22"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
+      <c r="E28" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>99</v>
+      </c>
       <c r="I28" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="22">
+    <row r="29" spans="1:9" ht="148.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="11">
         <v>24</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>100</v>
+      </c>
       <c r="I29" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="128.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="22">
+    <row r="30" spans="1:9" ht="134.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="11">
         <v>25</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="28" t="s">
+      <c r="B30" s="21"/>
+      <c r="C30" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="29" t="s">
+      <c r="D30" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="E30" s="22"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
+      <c r="E30" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12">
+        <v>23000</v>
+      </c>
+      <c r="H30" s="12">
+        <v>23000</v>
+      </c>
       <c r="I30" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="128.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="22">
+    <row r="31" spans="1:9" ht="130" x14ac:dyDescent="0.3">
+      <c r="A31" s="11">
         <v>26</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="28" t="s">
+      <c r="B31" s="21"/>
+      <c r="C31" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="29" t="s">
+      <c r="D31" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="E31" s="22"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
+      <c r="E31" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12">
+        <v>3</v>
+      </c>
+      <c r="H31" s="12">
+        <v>3</v>
+      </c>
       <c r="I31" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="39" x14ac:dyDescent="0.25">
-      <c r="A32" s="22">
+    <row r="32" spans="1:9" ht="65" x14ac:dyDescent="0.3">
+      <c r="A32" s="11">
         <v>27</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="28" t="s">
+      <c r="B32" s="21"/>
+      <c r="C32" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E32" s="22"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
+      <c r="E32" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>105</v>
+      </c>
       <c r="I32" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="39" x14ac:dyDescent="0.25">
-      <c r="A33" s="22">
+    <row r="33" spans="1:9" ht="39" x14ac:dyDescent="0.3">
+      <c r="A33" s="11">
         <v>28</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="28" t="s">
+      <c r="B33" s="21"/>
+      <c r="C33" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D33" s="29" t="s">
+      <c r="D33" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="E33" s="22"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
+      <c r="E33" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>103</v>
+      </c>
       <c r="I33" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="22">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="11">
         <v>29</v>
       </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="31" t="s">
+      <c r="B34" s="21"/>
+      <c r="C34" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="25" t="s">
+      <c r="D34" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="E34" s="22"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
+      <c r="E34" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>111</v>
+      </c>
       <c r="I34" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="22">
+    <row r="35" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="11">
         <v>30</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>112</v>
+      </c>
       <c r="I35" s="6" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="B6:B24"/>
-    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="B25:B35"/>
     <mergeCell ref="D34:D35"/>
     <mergeCell ref="D25:D27"/>
     <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B6:B24"/>
+    <mergeCell ref="C25:C27"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="D9:D12"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="D13:D16"/>
     <mergeCell ref="C19:C20"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>